<commit_message>
cleaned up, file now opens automatically
</commit_message>
<xml_diff>
--- a/extra_output.xlsx
+++ b/extra_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -25,55 +25,25 @@
     <t>retweets_count</t>
   </si>
   <si>
-    <t>nolanews</t>
-  </si>
-  <si>
-    <t>eaglebckim</t>
-  </si>
-  <si>
-    <t>afterprohibends</t>
-  </si>
-  <si>
-    <t>virginiaalee</t>
-  </si>
-  <si>
-    <t>alfredyegon12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Police found more than a dozen gummy products that said they contained CBD but instead had the dangerous street drug commonly known as K2 or spice.  https://buff.ly/2O4qJMA </t>
-  </si>
-  <si>
-    <t>$DCGD, already heading to big boom for 25Bil merger CBD banking and distribution, 42Mil low float soon to be locked again for $ 300-500.00, this week target will be $15.00, Max. based on news coming.  https://twitter.com/computerbux/status/1173945195613892608 …</t>
-  </si>
-  <si>
-    <t>Always liked the Green Party but I do find @GreenDrugPolicy somewhat confused  On one hand 'dont legalise cannabis that has less that 1% CBD to reduce risk from possible psychosis'  On the other It's 'lets legalise cocaine'  Why treat cannabis in a harsher manner than cocaine?  pic.twitter.com/nxZoaoekU1</t>
-  </si>
-  <si>
-    <t>.@brightfieldgrp’s Managing Director Bethany Gomez will be speaking on “The Future of CBD-Based Products” at @Groceryshop on 9/18.  https://groceryshop.com/speakers/125/bethany-gomez …. #groceryshop19 #CBD #grocery #mrx #retail</t>
-  </si>
-  <si>
-    <t>Nku cbd well represented @MunaiGenerali @sellyamutabi #driveonreloaded</t>
+    <t>bfs2020</t>
+  </si>
+  <si>
+    <t>craigcavyleader</t>
+  </si>
+  <si>
+    <t>MAGA2020 and Beyond....BLOCKED! @ MAGA4TRUMP2024 Here to piss off a few people! This page gives absolutely 0 Fucks, so nip it in the bud &amp; don’t debate me,got me!? #Lesbian #CBD #MAGA #WWG1WGA Lake Worth, TXJoined September 2018</t>
+  </si>
+  <si>
+    <t>someone explain why there's an advertisement in Queen St station telling people to "choose hope" by stopping taking antidepressants and instead taking up CBD oil, please</t>
   </si>
   <si>
     <t>likes_count</t>
   </si>
   <si>
-    <t>0amyque9c4cbddz</t>
-  </si>
-  <si>
-    <t>notpotdealer</t>
-  </si>
-  <si>
-    <t>cbdaiueermi3ngx</t>
-  </si>
-  <si>
-    <t>#さゆりんご #可愛く撮って ちょっと頑張って100いいね 目指してみます…🍎 さゆりん推し頼みます👸✨ pic.twitter.com/5URpsMcjtg</t>
-  </si>
-  <si>
-    <t>cultural impact:             █          　　            █　                    █　                    █　                          ＿          CBD                      essential       gummies               oil pyramid                                        schemes</t>
-  </si>
-  <si>
-    <t>ファボリツでお迎え  #美男美女さんと繋がりたい #らぶりつください #メンヘラ #ヤンデレ #病み垢さんいいね #お友達になりませんか #美男美女と繋がりたい #メンヘラさんと繋がりたい #らぶりつから気になった人お迎え #病み垢さんと繋がりたい #大切さん欲しい #私だけを見て #裏垢男子 #裏垢女子 pic.twitter.com/9DTCLRXfSJ</t>
+    <t>kickcbd</t>
+  </si>
+  <si>
+    <t>Officially 1 month until the Call of Duty: #ModernWarfare release!   #TeamKick pic.twitter.com/4ocmMWOjBo</t>
   </si>
   <si>
     <t>Username</t>
@@ -82,31 +52,37 @@
     <t>Number of Tweets</t>
   </si>
   <si>
-    <t>aicerabi</t>
+    <t>buyiegaimeds</t>
   </si>
   <si>
     <t>mmpconnect</t>
   </si>
   <si>
-    <t>budfoxfun</t>
-  </si>
-  <si>
-    <t>otcprwire</t>
+    <t>latisullivan</t>
   </si>
   <si>
     <t>aheadsocially</t>
   </si>
   <si>
+    <t>naturiciouscbd</t>
+  </si>
+  <si>
     <t>Date created:</t>
   </si>
   <si>
     <t>Time created:</t>
   </si>
   <si>
-    <t>17/09/2019</t>
-  </si>
-  <si>
-    <t>14:16:49</t>
+    <t>2019-09-25</t>
+  </si>
+  <si>
+    <t>17:59:59</t>
+  </si>
+  <si>
+    <t>Tweet Counter:</t>
+  </si>
+  <si>
+    <t>There are 3824 tweets in this document.</t>
   </si>
   <si>
     <t>Top 5 Retweeted</t>
@@ -193,7 +169,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -483,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,149 +492,135 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="2" t="s">
-        <v>31</v>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
       <c r="D10">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -647,66 +628,103 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="D21">
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B18:D23">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(B18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:D32">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:D14">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>